<commit_message>
Added Speedup Data for Lab Computer
</commit_message>
<xml_diff>
--- a/Documentation/Report/Results/Speedup_Timing.xlsx
+++ b/Documentation/Report/Results/Speedup_Timing.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="20352"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11010"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\n9763686\Documents\CVTree-Parallelised\Documentation\Report\Results\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jameskelly/Documents/Projects/CVTree-Parallelised/Documentation/Report/Results/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{37E47028-E8A1-4412-9813-8B4F2A8545BC}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4FCDB28E-C089-9C46-B1E8-23BA307A9B1B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="375" yWindow="495" windowWidth="28035" windowHeight="16500" xr2:uid="{8CECA080-1259-FD4C-8BBB-ABD117BA992B}"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="16500" xr2:uid="{8CECA080-1259-FD4C-8BBB-ABD117BA992B}"/>
   </bookViews>
   <sheets>
     <sheet name="QUT G-Lab Computer" sheetId="1" r:id="rId1"/>
@@ -20,12 +20,21 @@
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
     </ext>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+      </xcalcf:calcFeatures>
+    </ext>
   </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="20" uniqueCount="5">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9" uniqueCount="7">
   <si>
     <t>Test</t>
   </si>
@@ -40,6 +49,12 @@
   </si>
   <si>
     <t>Average</t>
+  </si>
+  <si>
+    <t>Speedup</t>
+  </si>
+  <si>
+    <t>N/A</t>
   </si>
 </sst>
 </file>
@@ -174,6 +189,1024 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/charts/chart1.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+  <c:date1904 val="0"/>
+  <c:lang val="en-GB"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="en-GB"/>
+              <a:t>Speedup Curve |</a:t>
+            </a:r>
+            <a:r>
+              <a:rPr lang="en-GB" baseline="0"/>
+              <a:t> CVTree Parallelised</a:t>
+            </a:r>
+            <a:endParaRPr lang="en-GB"/>
+          </a:p>
+        </c:rich>
+      </c:tx>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:lineChart>
+        <c:grouping val="stacked"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:spPr>
+            <a:ln w="28575" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent6"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="circle"/>
+            <c:size val="5"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent6"/>
+              </a:solidFill>
+              <a:ln w="9525">
+                <a:solidFill>
+                  <a:schemeClr val="accent6"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:marker>
+          <c:dLbls>
+            <c:spPr>
+              <a:noFill/>
+              <a:ln>
+                <a:noFill/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+            <c:txPr>
+              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" lIns="38100" tIns="19050" rIns="38100" bIns="19050" anchor="ctr" anchorCtr="1">
+                <a:spAutoFit/>
+              </a:bodyPr>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="75000"/>
+                        <a:lumOff val="25000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:endParaRPr lang="en-US"/>
+              </a:p>
+            </c:txPr>
+            <c:dLblPos val="t"/>
+            <c:showLegendKey val="0"/>
+            <c:showVal val="1"/>
+            <c:showCatName val="0"/>
+            <c:showSerName val="0"/>
+            <c:showPercent val="0"/>
+            <c:showBubbleSize val="0"/>
+            <c:showLeaderLines val="0"/>
+            <c:extLst>
+              <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
+                <c15:showLeaderLines val="1"/>
+                <c15:leaderLines>
+                  <c:spPr>
+                    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+                      <a:solidFill>
+                        <a:schemeClr val="tx1">
+                          <a:lumMod val="35000"/>
+                          <a:lumOff val="65000"/>
+                        </a:schemeClr>
+                      </a:solidFill>
+                      <a:round/>
+                    </a:ln>
+                    <a:effectLst/>
+                  </c:spPr>
+                </c15:leaderLines>
+              </c:ext>
+            </c:extLst>
+          </c:dLbls>
+          <c:val>
+            <c:numRef>
+              <c:f>'QUT G-Lab Computer'!$B$30:$B$37</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="8"/>
+                <c:pt idx="0">
+                  <c:v>0.95</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>1.8965000000000001</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>2.5626000000000002</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>3.0992000000000002</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>3.3816000000000002</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>3.6453000000000002</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>3.7448999999999999</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>3.8734999999999999</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000009-DE25-A041-871C-EFBDC3C5370B}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:dLbls>
+          <c:dLblPos val="t"/>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="1"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:marker val="1"/>
+        <c:smooth val="0"/>
+        <c:axId val="2100277023"/>
+        <c:axId val="2105061295"/>
+      </c:lineChart>
+      <c:catAx>
+        <c:axId val="2100277023"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:title>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1">
+                      <a:lumMod val="65000"/>
+                      <a:lumOff val="35000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="en-US"/>
+            </a:p>
+          </c:txPr>
+        </c:title>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="15000"/>
+                <a:lumOff val="85000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="2105061295"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+        <c:noMultiLvlLbl val="0"/>
+      </c:catAx>
+      <c:valAx>
+        <c:axId val="2105061295"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:title>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1">
+                      <a:lumMod val="65000"/>
+                      <a:lumOff val="35000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="en-US"/>
+            </a:p>
+          </c:txPr>
+        </c:title>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln>
+            <a:noFill/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="2100277023"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="between"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="zero"/>
+    <c:extLst>
+      <c:ext xmlns:c16r3="http://schemas.microsoft.com/office/drawing/2017/03/chart" uri="{56B9EC1D-385E-4148-901F-78D8002777C0}">
+        <c16r3:dataDisplayOptions16>
+          <c16r3:dispNaAsBlank val="1"/>
+        </c16r3:dataDisplayOptions16>
+      </c:ext>
+    </c:extLst>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="bg1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="tx1">
+          <a:lumMod val="15000"/>
+          <a:lumOff val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="en-US"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/colors1.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="13">
+  <a:schemeClr val="accent6"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent4"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
+<file path=xl/charts/style1.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="332">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:categoryAxis>
+  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="bg1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="28575" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="65000"/>
+          <a:lumOff val="35000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="5000"/>
+            <a:lumOff val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="75000"/>
+            <a:lumOff val="25000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1400" b="0" kern="1200" spc="0" baseline="0"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:prstDash val="sysDot"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
+<file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>57150</xdr:colOff>
+      <xdr:row>18</xdr:row>
+      <xdr:rowOff>63500</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>12</xdr:col>
+      <xdr:colOff>622300</xdr:colOff>
+      <xdr:row>37</xdr:row>
+      <xdr:rowOff>177800</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="2" name="Chart 1">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{C7536845-2C27-1E45-8A46-C40854294192}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -473,15 +1506,15 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1F6F1CE1-6E0C-934C-9DEE-40C6C81B6473}">
-  <dimension ref="A2:J15"/>
+  <dimension ref="A2:J37"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C20" sqref="C20"/>
+    <sheetView tabSelected="1" topLeftCell="A8" zoomScale="92" workbookViewId="0">
+      <selection activeCell="K44" sqref="K44"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <sheetData>
-    <row r="2" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A2" s="8" t="s">
         <v>3</v>
       </c>
@@ -495,7 +1528,7 @@
       <c r="I2" s="8"/>
       <c r="J2" s="8"/>
     </row>
-    <row r="3" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A3" s="2" t="s">
         <v>1</v>
       </c>
@@ -527,7 +1560,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="4" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A4" s="4" t="s">
         <v>0</v>
       </c>
@@ -541,7 +1574,7 @@
       <c r="I4" s="5"/>
       <c r="J4" s="5"/>
     </row>
-    <row r="5" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A5" s="4">
         <v>1</v>
       </c>
@@ -554,14 +1587,26 @@
       <c r="D5" s="1">
         <v>10.0667879</v>
       </c>
-      <c r="E5" s="1"/>
-      <c r="F5" s="1"/>
-      <c r="G5" s="1"/>
-      <c r="H5" s="1"/>
-      <c r="I5" s="1"/>
-      <c r="J5" s="1"/>
-    </row>
-    <row r="6" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="E5" s="1">
+        <v>7.6308629000000003</v>
+      </c>
+      <c r="F5" s="1">
+        <v>6.2746521</v>
+      </c>
+      <c r="G5" s="1">
+        <v>5.6915329000000003</v>
+      </c>
+      <c r="H5" s="1">
+        <v>5.3367756999999996</v>
+      </c>
+      <c r="I5" s="1">
+        <v>5.1821032000000002</v>
+      </c>
+      <c r="J5" s="1">
+        <v>4.9713425999999998</v>
+      </c>
+    </row>
+    <row r="6" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A6" s="4">
         <v>2</v>
       </c>
@@ -574,14 +1619,26 @@
       <c r="D6" s="1">
         <v>9.9179200000000005</v>
       </c>
-      <c r="E6" s="1"/>
-      <c r="F6" s="1"/>
-      <c r="G6" s="1"/>
-      <c r="H6" s="1"/>
-      <c r="I6" s="1"/>
-      <c r="J6" s="1"/>
-    </row>
-    <row r="7" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="E6" s="1">
+        <v>7.3837630000000001</v>
+      </c>
+      <c r="F6" s="1">
+        <v>6.0315099999999999</v>
+      </c>
+      <c r="G6" s="1">
+        <v>5.4774995000000004</v>
+      </c>
+      <c r="H6" s="1">
+        <v>5.1205034999999999</v>
+      </c>
+      <c r="I6" s="1">
+        <v>4.9794891000000003</v>
+      </c>
+      <c r="J6" s="1">
+        <v>4.7303642000000004</v>
+      </c>
+    </row>
+    <row r="7" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A7" s="4">
         <v>3</v>
       </c>
@@ -594,14 +1651,26 @@
       <c r="D7" s="1">
         <v>9.9467666000000001</v>
       </c>
-      <c r="E7" s="1"/>
-      <c r="F7" s="1"/>
-      <c r="G7" s="1"/>
-      <c r="H7" s="1"/>
-      <c r="I7" s="1"/>
-      <c r="J7" s="1"/>
-    </row>
-    <row r="8" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="E7" s="1">
+        <v>7.4234144999999998</v>
+      </c>
+      <c r="F7" s="1">
+        <v>6.2251390999999998</v>
+      </c>
+      <c r="G7" s="1">
+        <v>5.7702774000000003</v>
+      </c>
+      <c r="H7" s="1">
+        <v>5.3506894999999997</v>
+      </c>
+      <c r="I7" s="1">
+        <v>5.1927852999999997</v>
+      </c>
+      <c r="J7" s="1">
+        <v>5.0189494999999997</v>
+      </c>
+    </row>
+    <row r="8" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A8" s="4">
         <v>4</v>
       </c>
@@ -614,14 +1683,26 @@
       <c r="D8" s="1">
         <v>9.9654567000000007</v>
       </c>
-      <c r="E8" s="1"/>
-      <c r="F8" s="1"/>
-      <c r="G8" s="1"/>
-      <c r="H8" s="1"/>
-      <c r="I8" s="1"/>
-      <c r="J8" s="1"/>
-    </row>
-    <row r="9" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="E8" s="1">
+        <v>7.2585743999999996</v>
+      </c>
+      <c r="F8" s="1">
+        <v>6.0189031000000002</v>
+      </c>
+      <c r="G8" s="1">
+        <v>5.4715161999999999</v>
+      </c>
+      <c r="H8" s="1">
+        <v>5.1188529999999997</v>
+      </c>
+      <c r="I8" s="1">
+        <v>4.9484311999999999</v>
+      </c>
+      <c r="J8" s="1">
+        <v>4.7447169000000002</v>
+      </c>
+    </row>
+    <row r="9" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A9" s="4">
         <v>5</v>
       </c>
@@ -634,14 +1715,26 @@
       <c r="D9" s="1">
         <v>9.9849023999999993</v>
       </c>
-      <c r="E9" s="1"/>
-      <c r="F9" s="1"/>
-      <c r="G9" s="1"/>
-      <c r="H9" s="1"/>
-      <c r="I9" s="1"/>
-      <c r="J9" s="1"/>
-    </row>
-    <row r="10" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="E9" s="1">
+        <v>7.5666789999999997</v>
+      </c>
+      <c r="F9" s="1">
+        <v>6.2488124000000003</v>
+      </c>
+      <c r="G9" s="1">
+        <v>5.8853688999999996</v>
+      </c>
+      <c r="H9" s="1">
+        <v>5.2759283999999997</v>
+      </c>
+      <c r="I9" s="1">
+        <v>5.2247355999999998</v>
+      </c>
+      <c r="J9" s="1">
+        <v>5.0482120000000004</v>
+      </c>
+    </row>
+    <row r="10" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A10" s="4">
         <v>6</v>
       </c>
@@ -654,14 +1747,26 @@
       <c r="D10" s="1">
         <v>10.0197912</v>
       </c>
-      <c r="E10" s="1"/>
-      <c r="F10" s="1"/>
-      <c r="G10" s="1"/>
-      <c r="H10" s="1"/>
-      <c r="I10" s="1"/>
-      <c r="J10" s="1"/>
-    </row>
-    <row r="11" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="E10" s="1">
+        <v>7.3755158999999999</v>
+      </c>
+      <c r="F10" s="1">
+        <v>6.0782295</v>
+      </c>
+      <c r="G10" s="1">
+        <v>5.623259</v>
+      </c>
+      <c r="H10" s="1">
+        <v>5.1740008</v>
+      </c>
+      <c r="I10" s="1">
+        <v>4.9690994000000002</v>
+      </c>
+      <c r="J10" s="1">
+        <v>4.8978675000000003</v>
+      </c>
+    </row>
+    <row r="11" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A11" s="4">
         <v>7</v>
       </c>
@@ -674,14 +1779,26 @@
       <c r="D11" s="1">
         <v>10.0472965</v>
       </c>
-      <c r="E11" s="1"/>
-      <c r="F11" s="1"/>
-      <c r="G11" s="1"/>
-      <c r="H11" s="1"/>
-      <c r="I11" s="1"/>
-      <c r="J11" s="1"/>
-    </row>
-    <row r="12" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="E11" s="1">
+        <v>7.6615602000000003</v>
+      </c>
+      <c r="F11" s="1">
+        <v>6.1843127000000004</v>
+      </c>
+      <c r="G11" s="1">
+        <v>5.6464505000000003</v>
+      </c>
+      <c r="H11" s="1">
+        <v>5.3383396000000003</v>
+      </c>
+      <c r="I11" s="1">
+        <v>5.2318486000000002</v>
+      </c>
+      <c r="J11" s="1">
+        <v>5.008972</v>
+      </c>
+    </row>
+    <row r="12" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A12" s="4">
         <v>8</v>
       </c>
@@ -694,14 +1811,26 @@
       <c r="D12" s="1">
         <v>10.1000058</v>
       </c>
-      <c r="E12" s="1"/>
-      <c r="F12" s="1"/>
-      <c r="G12" s="1"/>
-      <c r="H12" s="1"/>
-      <c r="I12" s="1"/>
-      <c r="J12" s="1"/>
-    </row>
-    <row r="13" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="E12" s="1">
+        <v>7.3562604</v>
+      </c>
+      <c r="F12" s="1">
+        <v>6.0916082999999999</v>
+      </c>
+      <c r="G12" s="1">
+        <v>5.5099564000000001</v>
+      </c>
+      <c r="H12" s="1">
+        <v>5.1637842000000003</v>
+      </c>
+      <c r="I12" s="1">
+        <v>4.9451267000000003</v>
+      </c>
+      <c r="J12" s="1">
+        <v>4.8144806999999998</v>
+      </c>
+    </row>
+    <row r="13" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A13" s="4">
         <v>9</v>
       </c>
@@ -714,14 +1843,26 @@
       <c r="D13" s="1">
         <v>10.153045000000001</v>
       </c>
-      <c r="E13" s="1"/>
-      <c r="F13" s="1"/>
-      <c r="G13" s="1"/>
-      <c r="H13" s="1"/>
-      <c r="I13" s="1"/>
-      <c r="J13" s="1"/>
-    </row>
-    <row r="14" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="E13" s="1">
+        <v>7.4631270000000001</v>
+      </c>
+      <c r="F13" s="1">
+        <v>6.2681804000000003</v>
+      </c>
+      <c r="G13" s="1">
+        <v>5.7152095000000003</v>
+      </c>
+      <c r="H13" s="1">
+        <v>5.3015267000000001</v>
+      </c>
+      <c r="I13" s="1">
+        <v>5.2321913000000002</v>
+      </c>
+      <c r="J13" s="1">
+        <v>5.0139851000000002</v>
+      </c>
+    </row>
+    <row r="14" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A14" s="4">
         <v>10</v>
       </c>
@@ -734,14 +1875,26 @@
       <c r="D14" s="1">
         <v>10.279731</v>
       </c>
-      <c r="E14" s="1"/>
-      <c r="F14" s="1"/>
-      <c r="G14" s="1"/>
-      <c r="H14" s="1"/>
-      <c r="I14" s="1"/>
-      <c r="J14" s="1"/>
-    </row>
-    <row r="15" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="E14" s="1">
+        <v>7.2448655000000004</v>
+      </c>
+      <c r="F14" s="1">
+        <v>6.0658602000000004</v>
+      </c>
+      <c r="G14" s="1">
+        <v>5.5611331000000002</v>
+      </c>
+      <c r="H14" s="1">
+        <v>5.0958896999999999</v>
+      </c>
+      <c r="I14" s="1">
+        <v>4.9797852999999996</v>
+      </c>
+      <c r="J14" s="1">
+        <v>4.9476607000000001</v>
+      </c>
+    </row>
+    <row r="15" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A15" s="6" t="s">
         <v>4</v>
       </c>
@@ -757,29 +1910,189 @@
         <f t="shared" ref="D15:I15" si="0">SUM(D5:D14)/COUNT(D5:D14)</f>
         <v>10.04817031</v>
       </c>
-      <c r="E15" s="7" t="e">
+      <c r="E15" s="7">
         <f t="shared" si="0"/>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="F15" s="7" t="e">
+        <v>7.4364622799999989</v>
+      </c>
+      <c r="F15" s="7">
         <f t="shared" si="0"/>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="G15" s="7" t="e">
+        <v>6.1487207799999997</v>
+      </c>
+      <c r="G15" s="7">
         <f t="shared" si="0"/>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="H15" s="7" t="e">
+        <v>5.63522034</v>
+      </c>
+      <c r="H15" s="7">
         <f t="shared" si="0"/>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="I15" s="7" t="e">
+        <v>5.2276291099999996</v>
+      </c>
+      <c r="I15" s="7">
         <f t="shared" si="0"/>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="J15" s="7" t="e">
+        <v>5.088559570000001</v>
+      </c>
+      <c r="J15" s="7">
         <f>SUM(J5:J14)/COUNT(J5:J14)</f>
-        <v>#DIV/0!</v>
+        <v>4.9196551199999998</v>
+      </c>
+    </row>
+    <row r="18" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A18" t="s">
+        <v>1</v>
+      </c>
+      <c r="B18" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="19" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A19" t="s">
+        <v>2</v>
+      </c>
+      <c r="B19" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="20" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A20">
+        <v>1</v>
+      </c>
+      <c r="B20">
+        <f>B15/C15</f>
+        <v>0.94998718121780834</v>
+      </c>
+    </row>
+    <row r="21" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A21">
+        <v>2</v>
+      </c>
+      <c r="B21">
+        <f>B15/D15</f>
+        <v>1.8964960387897725</v>
+      </c>
+    </row>
+    <row r="22" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A22">
+        <v>3</v>
+      </c>
+      <c r="B22">
+        <f>B15/E15</f>
+        <v>2.5625511799140064</v>
+      </c>
+    </row>
+    <row r="23" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A23">
+        <v>4</v>
+      </c>
+      <c r="B23">
+        <f>B15/F15</f>
+        <v>3.0992324862082938</v>
+      </c>
+    </row>
+    <row r="24" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A24">
+        <v>5</v>
+      </c>
+      <c r="B24">
+        <f>B15/G15</f>
+        <v>3.3816450893205001</v>
+      </c>
+    </row>
+    <row r="25" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A25">
+        <v>6</v>
+      </c>
+      <c r="B25">
+        <f>B15/H15</f>
+        <v>3.6453074212068577</v>
+      </c>
+    </row>
+    <row r="26" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A26">
+        <v>7</v>
+      </c>
+      <c r="B26">
+        <f>B15/I15</f>
+        <v>3.7449331049100789</v>
+      </c>
+    </row>
+    <row r="27" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A27">
+        <v>8</v>
+      </c>
+      <c r="B27">
+        <f>B15/J15</f>
+        <v>3.873506318060767</v>
+      </c>
+    </row>
+    <row r="30" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A30">
+        <v>1</v>
+      </c>
+      <c r="B30">
+        <f>ROUND(B20, 4)</f>
+        <v>0.95</v>
+      </c>
+    </row>
+    <row r="31" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A31">
+        <v>2</v>
+      </c>
+      <c r="B31">
+        <f t="shared" ref="B31:B41" si="1">ROUND(B21, 4)</f>
+        <v>1.8965000000000001</v>
+      </c>
+    </row>
+    <row r="32" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A32">
+        <v>3</v>
+      </c>
+      <c r="B32">
+        <f t="shared" si="1"/>
+        <v>2.5626000000000002</v>
+      </c>
+    </row>
+    <row r="33" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A33">
+        <v>4</v>
+      </c>
+      <c r="B33">
+        <f t="shared" si="1"/>
+        <v>3.0992000000000002</v>
+      </c>
+    </row>
+    <row r="34" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A34">
+        <v>5</v>
+      </c>
+      <c r="B34">
+        <f t="shared" si="1"/>
+        <v>3.3816000000000002</v>
+      </c>
+    </row>
+    <row r="35" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A35">
+        <v>6</v>
+      </c>
+      <c r="B35">
+        <f t="shared" si="1"/>
+        <v>3.6453000000000002</v>
+      </c>
+    </row>
+    <row r="36" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A36">
+        <v>7</v>
+      </c>
+      <c r="B36">
+        <f t="shared" si="1"/>
+        <v>3.7448999999999999</v>
+      </c>
+    </row>
+    <row r="37" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A37">
+        <v>8</v>
+      </c>
+      <c r="B37">
+        <f t="shared" si="1"/>
+        <v>3.8734999999999999</v>
       </c>
     </row>
   </sheetData>
@@ -788,5 +2101,6 @@
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
+  <drawing r:id="rId2"/>
 </worksheet>
 </file>
</xml_diff>